<commit_message>
modify GuoTai_N entrust import data template
</commit_message>
<xml_diff>
--- a/src/Presentation/CTM.Win/DataTemplate/Entrust/GuoTai_N.xlsx
+++ b/src/Presentation/CTM.Win/DataTemplate/Entrust/GuoTai_N.xlsx
@@ -14,69 +14,18 @@
   <sheets>
     <sheet name="当日委托--国泰普通" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>委托时间</t>
-  </si>
-  <si>
-    <t>证券代码</t>
-  </si>
-  <si>
-    <t>证券名称</t>
-  </si>
-  <si>
-    <t>操作</t>
-  </si>
-  <si>
-    <t>备注</t>
-  </si>
-  <si>
-    <t>委托数量</t>
-  </si>
-  <si>
-    <t>成交数量</t>
-  </si>
-  <si>
-    <t>成交金额</t>
-  </si>
-  <si>
-    <t>委托价格</t>
-  </si>
-  <si>
-    <t>成交均价</t>
-  </si>
-  <si>
-    <t>合同编号</t>
-  </si>
-  <si>
-    <t>买入</t>
-  </si>
-  <si>
-    <t>冠豪高新</t>
-  </si>
-  <si>
-    <t>已成</t>
-  </si>
-  <si>
-    <t>亚星锚链</t>
-  </si>
-  <si>
-    <t>卖出</t>
-  </si>
-  <si>
-    <t>江特电机</t>
+    <t>交易类别</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>日内</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>交易类别</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -678,11 +627,8 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1040,164 +986,244 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" t="str">
+        <f>"委托日期"</f>
+        <v>委托日期</v>
+      </c>
+      <c r="B1" t="str">
+        <f>"委托时间"</f>
+        <v>委托时间</v>
+      </c>
+      <c r="C1" t="str">
+        <f>"证券代码"</f>
+        <v>证券代码</v>
+      </c>
+      <c r="D1" t="str">
+        <f>"证券名称"</f>
+        <v>证券名称</v>
+      </c>
+      <c r="E1" t="str">
+        <f>"买卖标志"</f>
+        <v>买卖标志</v>
+      </c>
+      <c r="F1" t="str">
+        <f>"委托价格"</f>
+        <v>委托价格</v>
+      </c>
+      <c r="G1" t="str">
+        <f>"委托数量"</f>
+        <v>委托数量</v>
+      </c>
+      <c r="H1" t="str">
+        <f>"委托编号"</f>
+        <v>委托编号</v>
+      </c>
+      <c r="I1" t="str">
+        <f>"成交数量"</f>
+        <v>成交数量</v>
+      </c>
+      <c r="J1" t="str">
+        <f>"撤单数量"</f>
+        <v>撤单数量</v>
+      </c>
+      <c r="K1" t="str">
+        <f>"状态说明"</f>
+        <v>状态说明</v>
+      </c>
+      <c r="L1" t="str">
+        <f>"撤单标志"</f>
+        <v>撤单标志</v>
+      </c>
+      <c r="M1" t="str">
+        <f>"股东代码"</f>
+        <v>股东代码</v>
+      </c>
+      <c r="N1" t="str">
+        <f>"操作日期"</f>
+        <v>操作日期</v>
+      </c>
+      <c r="O1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" t="str">
+        <f t="shared" ref="A2:A4" si="0">"20170301"</f>
+        <v>20170301</v>
+      </c>
+      <c r="B2" t="str">
+        <f>"14:34:37"</f>
+        <v>14:34:37</v>
+      </c>
+      <c r="C2" t="str">
+        <f t="shared" ref="C2:C4" si="1">"002798"</f>
+        <v>002798</v>
+      </c>
+      <c r="D2" t="str">
+        <f t="shared" ref="D2:D4" si="2">"帝王洁具"</f>
+        <v>帝王洁具</v>
+      </c>
+      <c r="E2" t="str">
+        <f t="shared" ref="E2:E4" si="3">"证券卖出"</f>
+        <v>证券卖出</v>
+      </c>
+      <c r="F2">
+        <v>58.35</v>
+      </c>
+      <c r="G2">
+        <v>4300</v>
+      </c>
+      <c r="H2" t="str">
+        <f>"270613"</f>
+        <v>270613</v>
+      </c>
+      <c r="I2">
+        <v>4300</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2" t="str">
+        <f>"已成"</f>
+        <v>已成</v>
+      </c>
+      <c r="L2" t="str">
+        <f t="shared" ref="L2:L4" si="4">"正常"</f>
+        <v>正常</v>
+      </c>
+      <c r="M2" t="str">
+        <f t="shared" ref="M2:M4" si="5">"0208635819"</f>
+        <v>0208635819</v>
+      </c>
+      <c r="N2" t="str">
+        <f t="shared" ref="N2:N4" si="6">"20170301"</f>
+        <v>20170301</v>
+      </c>
+      <c r="O2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>18</v>
-      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>0.56282407407407409</v>
-      </c>
-      <c r="B2">
-        <v>600433</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2">
-        <v>2000</v>
-      </c>
-      <c r="G2">
-        <v>2000</v>
-      </c>
-      <c r="H2">
-        <v>18960</v>
-      </c>
-      <c r="I2">
-        <v>9.48</v>
-      </c>
-      <c r="J2">
-        <v>9.48</v>
-      </c>
-      <c r="K2">
-        <v>156441</v>
-      </c>
-      <c r="L2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>0.41771990740740739</v>
-      </c>
-      <c r="B3">
-        <v>601890</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" t="str">
+        <f t="shared" si="0"/>
+        <v>20170301</v>
+      </c>
+      <c r="B3" t="str">
+        <f>"14:35:49"</f>
+        <v>14:35:49</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" si="1"/>
+        <v>002798</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" si="2"/>
+        <v>帝王洁具</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" si="3"/>
+        <v>证券卖出</v>
       </c>
       <c r="F3">
-        <v>2000</v>
+        <v>58.18</v>
       </c>
       <c r="G3">
         <v>2000</v>
       </c>
-      <c r="H3">
-        <v>20681.75</v>
+      <c r="H3" t="str">
+        <f>"271679"</f>
+        <v>271679</v>
       </c>
       <c r="I3">
-        <v>10.34</v>
+        <v>2000</v>
       </c>
       <c r="J3">
-        <v>10.340999999999999</v>
-      </c>
-      <c r="K3">
-        <v>66946</v>
-      </c>
-      <c r="L3" t="s">
-        <v>19</v>
+        <v>0</v>
+      </c>
+      <c r="K3" t="str">
+        <f>"已成"</f>
+        <v>已成</v>
+      </c>
+      <c r="L3" t="str">
+        <f t="shared" si="4"/>
+        <v>正常</v>
+      </c>
+      <c r="M3" t="str">
+        <f t="shared" si="5"/>
+        <v>0208635819</v>
+      </c>
+      <c r="N3" t="str">
+        <f t="shared" si="6"/>
+        <v>20170301</v>
+      </c>
+      <c r="O3" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>0.46460648148148148</v>
-      </c>
-      <c r="B4">
-        <v>2176</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" t="str">
+        <f t="shared" si="0"/>
+        <v>20170301</v>
+      </c>
+      <c r="B4" t="str">
+        <f>"14:37:59"</f>
+        <v>14:37:59</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="1"/>
+        <v>002798</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="2"/>
+        <v>帝王洁具</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="3"/>
+        <v>证券卖出</v>
       </c>
       <c r="F4">
-        <v>1400</v>
+        <v>58.58</v>
       </c>
       <c r="G4">
-        <v>1400</v>
-      </c>
-      <c r="H4">
-        <v>21644</v>
+        <v>8000</v>
+      </c>
+      <c r="H4" t="str">
+        <f>"273461"</f>
+        <v>273461</v>
       </c>
       <c r="I4">
-        <v>15.46</v>
+        <v>2800</v>
       </c>
       <c r="J4">
-        <v>15.46</v>
-      </c>
-      <c r="K4">
-        <v>122241</v>
-      </c>
-      <c r="L4" t="s">
-        <v>20</v>
+        <v>5200</v>
+      </c>
+      <c r="K4" t="str">
+        <f>"部撤"</f>
+        <v>部撤</v>
+      </c>
+      <c r="L4" t="str">
+        <f t="shared" si="4"/>
+        <v>正常</v>
+      </c>
+      <c r="M4" t="str">
+        <f t="shared" si="5"/>
+        <v>0208635819</v>
+      </c>
+      <c r="N4" t="str">
+        <f t="shared" si="6"/>
+        <v>20170301</v>
+      </c>
+      <c r="O4" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
MODIFY [GuoTai_N] ENTRUST TRADE DATA TEMPLATE
</commit_message>
<xml_diff>
--- a/src/Presentation/CTM.Win/DataTemplate/Entrust/GuoTai_N.xlsx
+++ b/src/Presentation/CTM.Win/DataTemplate/Entrust/GuoTai_N.xlsx
@@ -19,21 +19,69 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="20">
   <si>
     <t>交易类别</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>日内</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>波段</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>目标</t>
+    <t>委托时间</t>
+  </si>
+  <si>
+    <t>证券代码</t>
+  </si>
+  <si>
+    <t>证券名称</t>
+  </si>
+  <si>
+    <t>操作</t>
+  </si>
+  <si>
+    <t>备注</t>
+  </si>
+  <si>
+    <t>委托数量</t>
+  </si>
+  <si>
+    <t>成交数量</t>
+  </si>
+  <si>
+    <t>撤消数量</t>
+  </si>
+  <si>
+    <t>成交金额</t>
+  </si>
+  <si>
+    <t>委托价格</t>
+  </si>
+  <si>
+    <t>成交均价</t>
+  </si>
+  <si>
+    <t>合同编号</t>
+  </si>
+  <si>
+    <t>帝王洁具</t>
+  </si>
+  <si>
+    <t>证券买入</t>
+  </si>
+  <si>
+    <t>已成</t>
+  </si>
+  <si>
+    <t>部撤</t>
+  </si>
+  <si>
+    <t>波段</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>波段</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -627,8 +675,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -986,244 +1037,340 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+      <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" t="str">
-        <f>"委托日期"</f>
-        <v>委托日期</v>
-      </c>
-      <c r="B1" t="str">
-        <f>"委托时间"</f>
-        <v>委托时间</v>
-      </c>
-      <c r="C1" t="str">
-        <f>"证券代码"</f>
-        <v>证券代码</v>
-      </c>
-      <c r="D1" t="str">
-        <f>"证券名称"</f>
-        <v>证券名称</v>
-      </c>
-      <c r="E1" t="str">
-        <f>"买卖标志"</f>
-        <v>买卖标志</v>
-      </c>
-      <c r="F1" t="str">
-        <f>"委托价格"</f>
-        <v>委托价格</v>
-      </c>
-      <c r="G1" t="str">
-        <f>"委托数量"</f>
-        <v>委托数量</v>
-      </c>
-      <c r="H1" t="str">
-        <f>"委托编号"</f>
-        <v>委托编号</v>
-      </c>
-      <c r="I1" t="str">
-        <f>"成交数量"</f>
-        <v>成交数量</v>
-      </c>
-      <c r="J1" t="str">
-        <f>"撤单数量"</f>
-        <v>撤单数量</v>
-      </c>
-      <c r="K1" t="str">
-        <f>"状态说明"</f>
-        <v>状态说明</v>
-      </c>
-      <c r="L1" t="str">
-        <f>"撤单标志"</f>
-        <v>撤单标志</v>
-      </c>
-      <c r="M1" t="str">
-        <f>"股东代码"</f>
-        <v>股东代码</v>
-      </c>
-      <c r="N1" t="str">
-        <f>"操作日期"</f>
-        <v>操作日期</v>
-      </c>
-      <c r="O1" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" t="str">
-        <f t="shared" ref="A2:A4" si="0">"20170301"</f>
-        <v>20170301</v>
-      </c>
-      <c r="B2" t="str">
-        <f>"14:34:37"</f>
-        <v>14:34:37</v>
-      </c>
-      <c r="C2" t="str">
-        <f t="shared" ref="C2:C4" si="1">"002798"</f>
-        <v>002798</v>
-      </c>
-      <c r="D2" t="str">
-        <f t="shared" ref="D2:D4" si="2">"帝王洁具"</f>
-        <v>帝王洁具</v>
-      </c>
-      <c r="E2" t="str">
-        <f t="shared" ref="E2:E4" si="3">"证券卖出"</f>
-        <v>证券卖出</v>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>0.43079861111111112</v>
+      </c>
+      <c r="B2">
+        <v>2798</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
       </c>
       <c r="F2">
-        <v>58.35</v>
+        <v>4100</v>
       </c>
       <c r="G2">
-        <v>4300</v>
-      </c>
-      <c r="H2" t="str">
-        <f>"270613"</f>
-        <v>270613</v>
+        <v>4100</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
       </c>
       <c r="I2">
-        <v>4300</v>
+        <v>152900</v>
       </c>
       <c r="J2">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="K2">
+        <v>37.292999999999999</v>
+      </c>
+      <c r="L2">
+        <v>56987</v>
+      </c>
+      <c r="M2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>0.43062500000000004</v>
+      </c>
+      <c r="B3">
+        <v>2798</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3">
+        <v>8100</v>
+      </c>
+      <c r="G3">
+        <v>2600</v>
+      </c>
+      <c r="H3">
+        <v>5500</v>
+      </c>
+      <c r="I3">
+        <v>96555</v>
+      </c>
+      <c r="J3">
+        <v>37.15</v>
+      </c>
+      <c r="K3">
+        <v>37.137</v>
+      </c>
+      <c r="L3">
+        <v>56809</v>
+      </c>
+      <c r="M3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>0.43056712962962962</v>
+      </c>
+      <c r="B4">
+        <v>2798</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4">
+        <v>5100</v>
+      </c>
+      <c r="G4">
+        <v>5100</v>
+      </c>
+      <c r="H4">
         <v>0</v>
       </c>
-      <c r="K2" t="str">
-        <f>"已成"</f>
-        <v>已成</v>
-      </c>
-      <c r="L2" t="str">
-        <f t="shared" ref="L2:L4" si="4">"正常"</f>
-        <v>正常</v>
-      </c>
-      <c r="M2" t="str">
-        <f t="shared" ref="M2:M4" si="5">"0208635819"</f>
-        <v>0208635819</v>
-      </c>
-      <c r="N2" t="str">
-        <f t="shared" ref="N2:N4" si="6">"20170301"</f>
-        <v>20170301</v>
-      </c>
-      <c r="O2" t="s">
+      <c r="I4">
+        <v>189312</v>
+      </c>
+      <c r="J4">
+        <v>37.119999999999997</v>
+      </c>
+      <c r="K4">
+        <v>37.119999999999997</v>
+      </c>
+      <c r="L4">
+        <v>56755</v>
+      </c>
+      <c r="M4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" t="str">
-        <f t="shared" si="0"/>
-        <v>20170301</v>
-      </c>
-      <c r="B3" t="str">
-        <f>"14:35:49"</f>
-        <v>14:35:49</v>
-      </c>
-      <c r="C3" t="str">
-        <f t="shared" si="1"/>
-        <v>002798</v>
-      </c>
-      <c r="D3" t="str">
-        <f t="shared" si="2"/>
-        <v>帝王洁具</v>
-      </c>
-      <c r="E3" t="str">
-        <f t="shared" si="3"/>
-        <v>证券卖出</v>
-      </c>
-      <c r="F3">
-        <v>58.18</v>
-      </c>
-      <c r="G3">
-        <v>2000</v>
-      </c>
-      <c r="H3" t="str">
-        <f>"271679"</f>
-        <v>271679</v>
-      </c>
-      <c r="I3">
-        <v>2000</v>
-      </c>
-      <c r="J3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>0.4305208333333333</v>
+      </c>
+      <c r="B5">
+        <v>2798</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5">
+        <v>4100</v>
+      </c>
+      <c r="G5">
+        <v>3500</v>
+      </c>
+      <c r="H5">
+        <v>600</v>
+      </c>
+      <c r="I5">
+        <v>129885</v>
+      </c>
+      <c r="J5">
+        <v>37.11</v>
+      </c>
+      <c r="K5">
+        <v>37.11</v>
+      </c>
+      <c r="L5">
+        <v>56712</v>
+      </c>
+      <c r="M5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>0.43048611111111112</v>
+      </c>
+      <c r="B6">
+        <v>2798</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6">
+        <v>2100</v>
+      </c>
+      <c r="G6">
+        <v>2100</v>
+      </c>
+      <c r="H6">
         <v>0</v>
       </c>
-      <c r="K3" t="str">
-        <f>"已成"</f>
-        <v>已成</v>
-      </c>
-      <c r="L3" t="str">
-        <f t="shared" si="4"/>
-        <v>正常</v>
-      </c>
-      <c r="M3" t="str">
-        <f t="shared" si="5"/>
-        <v>0208635819</v>
-      </c>
-      <c r="N3" t="str">
-        <f t="shared" si="6"/>
-        <v>20170301</v>
-      </c>
-      <c r="O3" t="s">
-        <v>2</v>
+      <c r="I6">
+        <v>77931</v>
+      </c>
+      <c r="J6">
+        <v>37.11</v>
+      </c>
+      <c r="K6">
+        <v>37.11</v>
+      </c>
+      <c r="L6">
+        <v>56676</v>
+      </c>
+      <c r="M6" t="s">
+        <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" t="str">
-        <f t="shared" si="0"/>
-        <v>20170301</v>
-      </c>
-      <c r="B4" t="str">
-        <f>"14:37:59"</f>
-        <v>14:37:59</v>
-      </c>
-      <c r="C4" t="str">
-        <f t="shared" si="1"/>
-        <v>002798</v>
-      </c>
-      <c r="D4" t="str">
-        <f t="shared" si="2"/>
-        <v>帝王洁具</v>
-      </c>
-      <c r="E4" t="str">
-        <f t="shared" si="3"/>
-        <v>证券卖出</v>
-      </c>
-      <c r="F4">
-        <v>58.58</v>
-      </c>
-      <c r="G4">
-        <v>8000</v>
-      </c>
-      <c r="H4" t="str">
-        <f>"273461"</f>
-        <v>273461</v>
-      </c>
-      <c r="I4">
-        <v>2800</v>
-      </c>
-      <c r="J4">
-        <v>5200</v>
-      </c>
-      <c r="K4" t="str">
-        <f>"部撤"</f>
-        <v>部撤</v>
-      </c>
-      <c r="L4" t="str">
-        <f t="shared" si="4"/>
-        <v>正常</v>
-      </c>
-      <c r="M4" t="str">
-        <f t="shared" si="5"/>
-        <v>0208635819</v>
-      </c>
-      <c r="N4" t="str">
-        <f t="shared" si="6"/>
-        <v>20170301</v>
-      </c>
-      <c r="O4" t="s">
-        <v>3</v>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>0.4304398148148148</v>
+      </c>
+      <c r="B7">
+        <v>2798</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7">
+        <v>1400</v>
+      </c>
+      <c r="G7">
+        <v>1400</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>51954</v>
+      </c>
+      <c r="J7">
+        <v>37.11</v>
+      </c>
+      <c r="K7">
+        <v>37.11</v>
+      </c>
+      <c r="L7">
+        <v>56637</v>
+      </c>
+      <c r="M7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>0.43089120370370365</v>
+      </c>
+      <c r="B8">
+        <v>2798</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8">
+        <v>5100</v>
+      </c>
+      <c r="G8">
+        <v>5100</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>190725</v>
+      </c>
+      <c r="J8">
+        <v>37.479999999999997</v>
+      </c>
+      <c r="K8">
+        <v>37.396999999999998</v>
+      </c>
+      <c r="L8">
+        <v>57070</v>
+      </c>
+      <c r="M8" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>